<commit_message>
updated TODO.xlsx file and open reply under chosen message
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaha\Documents\github\final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFE67E2-B2FD-4D68-A2D6-97E6646B24D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DBBBFA-4BF7-43F3-B967-EAE079FF4AC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28965" yWindow="1560" windowWidth="16575" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="62">
   <si>
     <t>Task</t>
   </si>
@@ -187,13 +187,37 @@
   </si>
   <si>
     <t>update clicked message status in db</t>
+  </si>
+  <si>
+    <t>calendary date</t>
+  </si>
+  <si>
+    <t>add 'clicked' field to message class</t>
+  </si>
+  <si>
+    <t>28.3-3.4</t>
+  </si>
+  <si>
+    <t>21.3-27.3</t>
+  </si>
+  <si>
+    <t>11.4-17.4</t>
+  </si>
+  <si>
+    <t>14.3-21.1</t>
+  </si>
+  <si>
+    <t>7.3-13.3</t>
+  </si>
+  <si>
+    <t>4.4-10.4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +228,12 @@
     <font>
       <sz val="36"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -277,7 +307,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -300,11 +330,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -319,57 +362,87 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -658,13 +731,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,22 +747,23 @@
     <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="6">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20">
         <v>35</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -710,857 +784,993 @@
       <c r="F2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="G2" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="17">
-        <v>5</v>
-      </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17" t="s">
+      <c r="C3" s="12">
+        <v>5</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="26">
         <v>12</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="G3" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="12">
         <v>4</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17" t="s">
+      <c r="D4" s="12"/>
+      <c r="E4" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="26">
         <v>15</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="G4" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="12">
         <v>2</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17" t="s">
+      <c r="D5" s="12"/>
+      <c r="E5" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="26">
         <v>15</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="G5" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="12">
         <v>2</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17" t="s">
+      <c r="D7" s="12"/>
+      <c r="E7" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="26">
         <v>15</v>
       </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="G7" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16" t="s">
+      <c r="A8" s="21"/>
+      <c r="B8" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="12">
         <v>3</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17" t="s">
+      <c r="D8" s="12"/>
+      <c r="E8" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="26">
         <v>15</v>
       </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="G8" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="12">
-        <v>5</v>
-      </c>
-      <c r="D10" s="12" t="s">
+      <c r="C10" s="8">
+        <v>5</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="28">
         <v>10</v>
       </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="G10" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="14">
         <v>4</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="29">
         <v>10</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="G11" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19"/>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="17">
-        <v>5</v>
-      </c>
-      <c r="D12" s="17" t="s">
+      <c r="C12" s="12">
+        <v>5</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="26">
         <v>10</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="G12" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="17">
-        <v>5</v>
-      </c>
-      <c r="D13" s="17" t="s">
+      <c r="C13" s="12">
+        <v>5</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="26">
         <v>10</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
+      <c r="G13" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="19"/>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="17">
-        <v>5</v>
-      </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17" t="s">
+      <c r="C14" s="12">
+        <v>5</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="26">
         <v>11</v>
       </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="G14" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="17">
-        <v>5</v>
-      </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17" t="s">
+      <c r="C15" s="12">
+        <v>5</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="26">
         <v>11</v>
       </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="G15" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="17">
-        <v>5</v>
-      </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17" t="s">
+      <c r="C16" s="12">
+        <v>5</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="26">
         <v>10</v>
       </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
+      <c r="G16" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="12">
+        <v>5</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="26">
+        <v>14</v>
+      </c>
+      <c r="G17" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="19"/>
+      <c r="B18" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="17">
-        <v>5</v>
-      </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17" t="s">
+      <c r="C18" s="12">
+        <v>5</v>
+      </c>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F18" s="26">
         <v>11</v>
       </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
+      <c r="G18" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="12">
-        <v>5</v>
-      </c>
-      <c r="D19" s="12" t="s">
+      <c r="C20" s="8">
+        <v>5</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E20" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F20" s="28">
         <v>10</v>
       </c>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="11" t="s">
+      <c r="G20" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
+      <c r="B21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C21" s="8">
         <v>4</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D21" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E21" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F21" s="28">
         <v>10</v>
       </c>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="11" t="s">
+      <c r="G21" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="22"/>
+      <c r="B22" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="12">
-        <v>5</v>
-      </c>
-      <c r="D21" s="12" t="s">
+      <c r="C22" s="8">
+        <v>5</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E22" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F22" s="28">
         <v>10</v>
       </c>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="16" t="s">
+      <c r="G22" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="22"/>
+      <c r="B23" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="17">
-        <v>5</v>
-      </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17" t="s">
+      <c r="C23" s="12">
+        <v>5</v>
+      </c>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F22" s="17">
+      <c r="F23" s="26">
         <v>12</v>
       </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="16" t="s">
+      <c r="G23" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="22"/>
+      <c r="B24" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="17">
-        <v>5</v>
-      </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="F23" s="17">
-        <v>12</v>
-      </c>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="11" t="s">
-        <v>22</v>
-      </c>
       <c r="C24" s="12">
-        <v>4</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>48</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D24" s="12"/>
       <c r="E24" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="26">
+        <v>12</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="22"/>
+      <c r="B25" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="8">
+        <v>4</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="28">
         <v>10</v>
       </c>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
-      <c r="B25" s="11" t="s">
+      <c r="G25" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="22"/>
+      <c r="B26" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="12">
-        <v>5</v>
-      </c>
-      <c r="D25" s="12" t="s">
+      <c r="C26" s="8">
+        <v>5</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E26" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F25" s="12">
+      <c r="F26" s="28">
         <v>10</v>
       </c>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
-      <c r="B26" s="13" t="s">
+      <c r="G26" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="22"/>
+      <c r="B27" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="14">
-        <v>5</v>
-      </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14" t="s">
+      <c r="C27" s="10">
+        <v>5</v>
+      </c>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F26" s="14">
+      <c r="F27" s="30">
         <v>13</v>
       </c>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="21"/>
-      <c r="B27" s="13" t="s">
+      <c r="G27" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="22"/>
+      <c r="B28" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="14">
-        <v>5</v>
-      </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14" t="s">
+      <c r="C28" s="10">
+        <v>5</v>
+      </c>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F27" s="14">
+      <c r="F28" s="30">
         <v>13</v>
       </c>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
-      <c r="B28" s="13" t="s">
+      <c r="G28" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="22"/>
+      <c r="B29" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="14">
-        <v>5</v>
-      </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14" t="s">
+      <c r="C29" s="8">
+        <v>5</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F28" s="14">
+      <c r="F29" s="28">
         <v>13</v>
       </c>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
-      <c r="B29" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="17">
-        <v>4</v>
-      </c>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="F29" s="17">
-        <v>13</v>
-      </c>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
+      <c r="G29" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-    </row>
-    <row r="31" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="23" t="s">
+      <c r="B30" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="12">
+        <v>4</v>
+      </c>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F30" s="26">
+        <v>13</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+    </row>
+    <row r="32" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B32" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="17">
+      <c r="C32" s="12">
         <v>2</v>
       </c>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17" t="s">
+      <c r="D32" s="12"/>
+      <c r="E32" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F31" s="17">
+      <c r="F32" s="26">
         <v>15</v>
       </c>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
-      <c r="B32" s="16" t="s">
+      <c r="G32" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="17"/>
+      <c r="B33" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="17">
+      <c r="C33" s="12">
         <v>3</v>
       </c>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17" t="s">
+      <c r="D33" s="12"/>
+      <c r="E33" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F32" s="17">
+      <c r="F33" s="26">
         <v>15</v>
       </c>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
-      <c r="B33" s="16" t="s">
+      <c r="G33" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="17"/>
+      <c r="B34" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="17">
+      <c r="C34" s="12">
         <v>3</v>
       </c>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17" t="s">
+      <c r="D34" s="12"/>
+      <c r="E34" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F33" s="17">
+      <c r="F34" s="26">
         <v>15</v>
       </c>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="23"/>
-      <c r="B34" s="16" t="s">
+      <c r="G34" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="17"/>
+      <c r="B35" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="17">
+      <c r="C35" s="12">
         <v>3</v>
       </c>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17" t="s">
+      <c r="D35" s="12"/>
+      <c r="E35" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F34" s="17">
+      <c r="F35" s="26">
         <v>15</v>
       </c>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
-      <c r="B35" s="16" t="s">
+      <c r="G35" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="17"/>
+      <c r="B36" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="17">
+      <c r="C36" s="12">
         <v>3</v>
       </c>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17" t="s">
+      <c r="D36" s="12"/>
+      <c r="E36" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F35" s="17">
+      <c r="F36" s="26">
         <v>15</v>
       </c>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
-      <c r="B36" s="16" t="s">
+      <c r="G36" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="17"/>
+      <c r="B37" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="17">
+      <c r="C37" s="12">
         <v>3</v>
       </c>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17" t="s">
+      <c r="D37" s="12"/>
+      <c r="E37" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F36" s="17">
+      <c r="F37" s="26">
         <v>15</v>
       </c>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
-      <c r="B37" s="16" t="s">
+      <c r="G37" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="17"/>
+      <c r="B38" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="17">
+      <c r="C38" s="12">
         <v>2</v>
       </c>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17" t="s">
+      <c r="D38" s="12"/>
+      <c r="E38" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F37" s="17">
+      <c r="F38" s="26">
         <v>15</v>
       </c>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="23"/>
-      <c r="B38" s="16" t="s">
+      <c r="G38" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="17"/>
+      <c r="B39" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="17">
+      <c r="C39" s="12">
         <v>2</v>
       </c>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17" t="s">
+      <c r="D39" s="12"/>
+      <c r="E39" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F38" s="17">
+      <c r="F39" s="26">
         <v>15</v>
       </c>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-    </row>
-    <row r="40" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
+      <c r="G39" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="16"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+    </row>
+    <row r="41" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="1">
-        <v>5</v>
-      </c>
-      <c r="E40" s="1" t="s">
+      <c r="B41" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="12">
+        <v>5</v>
+      </c>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F41" s="12">
         <v>12</v>
       </c>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="10"/>
-      <c r="B41" s="2" t="s">
+      <c r="G41" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="18"/>
+      <c r="B42" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C41" s="1">
-        <v>5</v>
-      </c>
-      <c r="E41" s="1" t="s">
+      <c r="C42" s="12">
+        <v>5</v>
+      </c>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F41" s="1">
+      <c r="F42" s="12">
         <v>12</v>
       </c>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="10"/>
-      <c r="B42" s="2" t="s">
+      <c r="G42" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="18"/>
+      <c r="B43" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="1">
-        <v>5</v>
-      </c>
-      <c r="E42" s="1" t="s">
+      <c r="C43" s="12">
+        <v>5</v>
+      </c>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F43" s="12">
         <v>12</v>
       </c>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="10"/>
-      <c r="B43" s="2" t="s">
+      <c r="G43" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="18"/>
+      <c r="B44" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C43" s="1">
-        <v>5</v>
-      </c>
-      <c r="E43" s="1" t="s">
+      <c r="C44" s="12">
+        <v>5</v>
+      </c>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F43" s="1">
+      <c r="F44" s="12">
         <v>12</v>
       </c>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="10"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="7"/>
+      <c r="G44" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="7"/>
+      <c r="A45" s="18"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="7"/>
+      <c r="A46" s="6"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="24"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
+      <c r="A47" s="6"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
-      <c r="I48" s="7"/>
-    </row>
-    <row r="49" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G49" s="7"/>
-      <c r="H49" s="7"/>
-      <c r="I49" s="7"/>
-    </row>
-    <row r="50" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G50" s="7"/>
-      <c r="H50" s="7"/>
-      <c r="I50" s="7"/>
-    </row>
-    <row r="51" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G51" s="7"/>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-    </row>
-    <row r="52" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G52" s="7"/>
-      <c r="H52" s="7"/>
-      <c r="I52" s="7"/>
-    </row>
-    <row r="53" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G53" s="7"/>
-      <c r="H53" s="7"/>
-      <c r="I53" s="7"/>
-    </row>
-    <row r="54" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G54" s="7"/>
-      <c r="H54" s="7"/>
-      <c r="I54" s="7"/>
-    </row>
-    <row r="55" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G55" s="7"/>
-      <c r="H55" s="7"/>
-      <c r="I55" s="7"/>
-    </row>
-    <row r="56" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G56" s="7"/>
-      <c r="H56" s="7"/>
-      <c r="I56" s="7"/>
-    </row>
-    <row r="57" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
-      <c r="I57" s="7"/>
+      <c r="A48" s="6"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="24"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="6"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="24"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G51" s="24"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G52" s="24"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G53" s="24"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G54" s="24"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G55" s="24"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G56" s="24"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G57" s="24"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G58" s="24"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A30:F30"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A31:A38"/>
-    <mergeCell ref="A40:A44"/>
-    <mergeCell ref="A10:A17"/>
+  <mergeCells count="11">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A3:A8"/>
-    <mergeCell ref="A19:A29"/>
+    <mergeCell ref="A20:A30"/>
     <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A32:A39"/>
+    <mergeCell ref="A41:A45"/>
+    <mergeCell ref="A10:A18"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update TODO list: add specification sheet
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaha\Documents\github\final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74763741-AB1B-4F6B-B67F-DBBD7EA81047}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB474BB-BD98-4DA7-9389-8EE2AB47CC2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29790" yWindow="1905" windowWidth="16035" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29790" yWindow="1905" windowWidth="23385" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ATP" sheetId="2" r:id="rId2"/>
+    <sheet name="specification" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$20:$G$31</definedName>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="106">
   <si>
     <t>Task</t>
   </si>
@@ -214,13 +216,145 @@
   </si>
   <si>
     <t>4.4-10.4</t>
+  </si>
+  <si>
+    <t>Acceptance Test Procedure</t>
+  </si>
+  <si>
+    <t>tested module</t>
+  </si>
+  <si>
+    <t>Req. ID</t>
+  </si>
+  <si>
+    <t>Precedure</t>
+  </si>
+  <si>
+    <t>module</t>
+  </si>
+  <si>
+    <t>requirement</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>user can subscribe to letter notification</t>
+  </si>
+  <si>
+    <t>web page showcases the company's products portfolio</t>
+  </si>
+  <si>
+    <t>web page showcases the company's main interest and business</t>
+  </si>
+  <si>
+    <t>web page showcases the company's contact avanues</t>
+  </si>
+  <si>
+    <t>web page showcases the company's example uses(project management, information sharing etc..)</t>
+  </si>
+  <si>
+    <t>user can purchase without sign-in procedure</t>
+  </si>
+  <si>
+    <t>user can purchase safely</t>
+  </si>
+  <si>
+    <t>user can sign-up to website</t>
+  </si>
+  <si>
+    <t>user can sign into website</t>
+  </si>
+  <si>
+    <t>website provides with administrator prevliges</t>
+  </si>
+  <si>
+    <t>admin can add product</t>
+  </si>
+  <si>
+    <t>admin can add user</t>
+  </si>
+  <si>
+    <t>admin can remove user</t>
+  </si>
+  <si>
+    <t>registered user can view past orders</t>
+  </si>
+  <si>
+    <t>registered user can place new order</t>
+  </si>
+  <si>
+    <t>admin can view all orders</t>
+  </si>
+  <si>
+    <t>registered user can start a new project</t>
+  </si>
+  <si>
+    <t>registered user can add new step(s) to a project</t>
+  </si>
+  <si>
+    <t>registered user can send messages(s) to other users</t>
+  </si>
+  <si>
+    <t>registered user can view all messages from any other users(s)</t>
+  </si>
+  <si>
+    <t>registered user can add comments to his\hers or other registered users projects</t>
+  </si>
+  <si>
+    <t>registered user can view personal details</t>
+  </si>
+  <si>
+    <t>registered user can edit personal details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin can mark users as 'expert', 'professional', 'amature', 'intern' </t>
+  </si>
+  <si>
+    <t>admin can add\remove suppliers</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>code version control must be used</t>
+  </si>
+  <si>
+    <t>build tool must be used</t>
+  </si>
+  <si>
+    <t>code should apply most efficient algorithms</t>
+  </si>
+  <si>
+    <t>deployment to both linux and windows platforms</t>
+  </si>
+  <si>
+    <t>code must employ separations of concerns paradigm</t>
+  </si>
+  <si>
+    <t>back end uses OOP</t>
+  </si>
+  <si>
+    <t>derived specifications</t>
+  </si>
+  <si>
+    <t>user is presented with 'log-in' form</t>
+  </si>
+  <si>
+    <t>upon successful registration user is redirected to 'user' page</t>
+  </si>
+  <si>
+    <t>registration to website under regular user privileges only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#requirement </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,8 +375,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -309,6 +450,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -350,7 +503,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -446,6 +599,77 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -736,11 +960,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E31" sqref="E31"/>
+      <selection pane="bottomRight" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1804,4 +2028,464 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A0F47E2-10A4-4971-BDBB-DDE68573EB84}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="7" width="19.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="46.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F1C7CD-19A3-4E4C-8995-F8BF8AD34968}">
+  <dimension ref="A2:D44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="61.5703125" customWidth="1"/>
+    <col min="4" max="4" width="70.7109375" style="36" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" s="34" customFormat="1" ht="46.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+    </row>
+    <row r="4" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="46">
+        <v>1</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="47" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="45"/>
+      <c r="B5" s="46">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C5" s="46"/>
+      <c r="D5" s="47" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="45"/>
+      <c r="B6" s="46">
+        <v>1.2</v>
+      </c>
+      <c r="C6" s="46"/>
+      <c r="D6" s="47" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="45"/>
+      <c r="B7" s="46">
+        <v>1.3</v>
+      </c>
+      <c r="C7" s="46"/>
+      <c r="D7" s="47" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="45"/>
+      <c r="B8" s="46">
+        <v>1.4</v>
+      </c>
+      <c r="C8" s="46"/>
+      <c r="D8" s="47" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="45"/>
+      <c r="B9" s="46">
+        <v>1.5</v>
+      </c>
+      <c r="C9" s="46"/>
+      <c r="D9" s="47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="45"/>
+      <c r="B10" s="46">
+        <v>1.6</v>
+      </c>
+      <c r="C10" s="46"/>
+      <c r="D10" s="47" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="45"/>
+      <c r="B11" s="46">
+        <v>1.7</v>
+      </c>
+      <c r="C11" s="46"/>
+      <c r="D11" s="47" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="45"/>
+      <c r="B12" s="46">
+        <v>1.8</v>
+      </c>
+      <c r="C12" s="46"/>
+      <c r="D12" s="47" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="45"/>
+      <c r="B13" s="48">
+        <v>2</v>
+      </c>
+      <c r="C13" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="47" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="45"/>
+      <c r="B14" s="48">
+        <v>2.1</v>
+      </c>
+      <c r="C14" s="50"/>
+      <c r="D14" s="47" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="45"/>
+      <c r="B15" s="48">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C15" s="50"/>
+      <c r="D15" s="47" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="45"/>
+      <c r="B16" s="48">
+        <v>3</v>
+      </c>
+      <c r="C16" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="47"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="45"/>
+      <c r="B17" s="48">
+        <v>3.1</v>
+      </c>
+      <c r="C17" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="47"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="45"/>
+      <c r="B18" s="48">
+        <v>3.2</v>
+      </c>
+      <c r="C18" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="47"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="45"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="47"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="37"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="52">
+        <v>4</v>
+      </c>
+      <c r="C21" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="54"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="51"/>
+      <c r="B22" s="52">
+        <v>5</v>
+      </c>
+      <c r="C22" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="54"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="51"/>
+      <c r="B23" s="52">
+        <v>6</v>
+      </c>
+      <c r="C23" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="54"/>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="51"/>
+      <c r="B24" s="52">
+        <v>7</v>
+      </c>
+      <c r="C24" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="54"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="51"/>
+      <c r="B25" s="52">
+        <v>8</v>
+      </c>
+      <c r="C25" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="54" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="51"/>
+      <c r="B26" s="52">
+        <v>8.1</v>
+      </c>
+      <c r="C26" s="53"/>
+      <c r="D26" s="54" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="51"/>
+      <c r="B27" s="52">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C27" s="53"/>
+      <c r="D27" s="54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="51"/>
+      <c r="B28" s="52">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="C28" s="53"/>
+      <c r="D28" s="54" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="51"/>
+      <c r="B29" s="52">
+        <v>8.4</v>
+      </c>
+      <c r="C29" s="53"/>
+      <c r="D29" s="54" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="51"/>
+      <c r="B30" s="52">
+        <v>8.5</v>
+      </c>
+      <c r="C30" s="53"/>
+      <c r="D30" s="54" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="38"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="40"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="55" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" s="56">
+        <v>9</v>
+      </c>
+      <c r="C32" s="57" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" s="58"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="55"/>
+      <c r="B33" s="56">
+        <v>10</v>
+      </c>
+      <c r="C33" s="57" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="58"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="55"/>
+      <c r="B34" s="56">
+        <v>11</v>
+      </c>
+      <c r="C34" s="57" t="s">
+        <v>97</v>
+      </c>
+      <c r="D34" s="58"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="55"/>
+      <c r="B35" s="56">
+        <v>12</v>
+      </c>
+      <c r="C35" s="57" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" s="58"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="55"/>
+      <c r="B36" s="56">
+        <v>13</v>
+      </c>
+      <c r="C36" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="D36" s="58"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="55"/>
+      <c r="B37" s="56">
+        <v>14</v>
+      </c>
+      <c r="C37" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" s="58"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="38"/>
+      <c r="B38" s="39"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="40"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="35"/>
+      <c r="C39" s="35"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="35"/>
+      <c r="C40" s="35"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="35"/>
+      <c r="C41" s="35"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="35"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="A4:A19"/>
+    <mergeCell ref="A21:A30"/>
+    <mergeCell ref="A20:D20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
reset message display field (remove user name from 'dislpay')
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaha\Documents\github\final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09853B6C-FD83-41AC-AEBA-FF9E45858442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07F3B02-A801-4805-9A89-6F1F6A54614D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="128">
   <si>
     <t>Task</t>
   </si>
@@ -402,6 +402,18 @@
   </si>
   <si>
     <t>user can hide messages</t>
+  </si>
+  <si>
+    <t>user cannot hide/delete 'admin' messages</t>
+  </si>
+  <si>
+    <t>only user that sent the message can delete it</t>
+  </si>
+  <si>
+    <t>user can hide message, thus it will not bedisplayed on user UI</t>
+  </si>
+  <si>
+    <t>user can see all hidden messages (as long as not deleted)</t>
   </si>
 </sst>
 </file>
@@ -692,6 +704,36 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -710,21 +752,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -737,23 +764,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1062,17 +1074,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48">
         <v>35</v>
       </c>
-      <c r="G1" s="49"/>
+      <c r="G1" s="48"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
     </row>
@@ -1102,7 +1114,7 @@
       <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="49" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -1125,7 +1137,7 @@
       <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="50"/>
+      <c r="A4" s="49"/>
       <c r="B4" s="11" t="s">
         <v>39</v>
       </c>
@@ -1146,7 +1158,7 @@
       <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="50"/>
+      <c r="A5" s="49"/>
       <c r="B5" s="11" t="s">
         <v>40</v>
       </c>
@@ -1167,7 +1179,7 @@
       <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="50"/>
+      <c r="A6" s="49"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
@@ -1178,7 +1190,7 @@
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="50"/>
+      <c r="A7" s="49"/>
       <c r="B7" s="11" t="s">
         <v>42</v>
       </c>
@@ -1199,7 +1211,7 @@
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
+      <c r="A8" s="49"/>
       <c r="B8" s="11" t="s">
         <v>41</v>
       </c>
@@ -1220,18 +1232,18 @@
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="53"/>
+      <c r="A9" s="51"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="52"/>
       <c r="G9" s="13"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="58" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -1256,7 +1268,7 @@
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="48"/>
+      <c r="A11" s="58"/>
       <c r="B11" s="7" t="s">
         <v>10</v>
       </c>
@@ -1279,7 +1291,7 @@
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
+      <c r="A12" s="58"/>
       <c r="B12" s="11" t="s">
         <v>12</v>
       </c>
@@ -1302,7 +1314,7 @@
       <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="48"/>
+      <c r="A13" s="58"/>
       <c r="B13" s="11" t="s">
         <v>13</v>
       </c>
@@ -1325,7 +1337,7 @@
       <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="48"/>
+      <c r="A14" s="58"/>
       <c r="B14" s="11" t="s">
         <v>14</v>
       </c>
@@ -1346,7 +1358,7 @@
       <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="48"/>
+      <c r="A15" s="58"/>
       <c r="B15" s="11" t="s">
         <v>15</v>
       </c>
@@ -1367,7 +1379,7 @@
       <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="48"/>
+      <c r="A16" s="58"/>
       <c r="B16" s="11" t="s">
         <v>7</v>
       </c>
@@ -1388,7 +1400,7 @@
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="48"/>
+      <c r="A17" s="58"/>
       <c r="B17" s="11" t="s">
         <v>55</v>
       </c>
@@ -1409,7 +1421,7 @@
       <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="48"/>
+      <c r="A18" s="58"/>
       <c r="B18" s="11" t="s">
         <v>16</v>
       </c>
@@ -1430,18 +1442,18 @@
       <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="52"/>
-      <c r="B19" s="52"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="53"/>
+      <c r="A19" s="51"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="52"/>
       <c r="G19" s="13"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="51" t="s">
+      <c r="A20" s="50" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -1466,7 +1478,7 @@
       <c r="I20" s="6"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
+      <c r="A21" s="50"/>
       <c r="B21" s="7" t="s">
         <v>18</v>
       </c>
@@ -1489,7 +1501,7 @@
       <c r="I21" s="6"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="51"/>
+      <c r="A22" s="50"/>
       <c r="B22" s="7" t="s">
         <v>19</v>
       </c>
@@ -1512,7 +1524,7 @@
       <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="51"/>
+      <c r="A23" s="50"/>
       <c r="B23" s="11" t="s">
         <v>20</v>
       </c>
@@ -1533,7 +1545,7 @@
       <c r="I23" s="6"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="51"/>
+      <c r="A24" s="50"/>
       <c r="B24" s="11" t="s">
         <v>21</v>
       </c>
@@ -1554,7 +1566,7 @@
       <c r="I24" s="6"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="51"/>
+      <c r="A25" s="50"/>
       <c r="B25" s="7" t="s">
         <v>22</v>
       </c>
@@ -1577,7 +1589,7 @@
       <c r="I25" s="6"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="51"/>
+      <c r="A26" s="50"/>
       <c r="B26" s="7" t="s">
         <v>8</v>
       </c>
@@ -1600,7 +1612,7 @@
       <c r="I26" s="6"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="51"/>
+      <c r="A27" s="50"/>
       <c r="B27" s="9" t="s">
         <v>51</v>
       </c>
@@ -1621,7 +1633,7 @@
       <c r="I27" s="6"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="51"/>
+      <c r="A28" s="50"/>
       <c r="B28" s="7" t="s">
         <v>53</v>
       </c>
@@ -1644,7 +1656,7 @@
       <c r="I28" s="6"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="51"/>
+      <c r="A29" s="50"/>
       <c r="B29" s="7" t="s">
         <v>52</v>
       </c>
@@ -1667,7 +1679,7 @@
       <c r="I29" s="6"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="51"/>
+      <c r="A30" s="50"/>
       <c r="B30" s="7" t="s">
         <v>42</v>
       </c>
@@ -1690,7 +1702,7 @@
       <c r="I30" s="6"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="51"/>
+      <c r="A31" s="50"/>
       <c r="B31" s="11" t="s">
         <v>23</v>
       </c>
@@ -1711,18 +1723,18 @@
       <c r="I31" s="6"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="43"/>
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="44"/>
+      <c r="A32" s="53"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="54"/>
       <c r="G32" s="13"/>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
     </row>
     <row r="33" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="46" t="s">
+      <c r="A33" s="56" t="s">
         <v>30</v>
       </c>
       <c r="B33" s="11" t="s">
@@ -1745,7 +1757,7 @@
       <c r="I33" s="6"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="46"/>
+      <c r="A34" s="56"/>
       <c r="B34" s="11" t="s">
         <v>25</v>
       </c>
@@ -1766,7 +1778,7 @@
       <c r="I34" s="6"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="46"/>
+      <c r="A35" s="56"/>
       <c r="B35" s="11" t="s">
         <v>26</v>
       </c>
@@ -1787,7 +1799,7 @@
       <c r="I35" s="6"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="46"/>
+      <c r="A36" s="56"/>
       <c r="B36" s="11" t="s">
         <v>27</v>
       </c>
@@ -1808,7 +1820,7 @@
       <c r="I36" s="6"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="46"/>
+      <c r="A37" s="56"/>
       <c r="B37" s="11" t="s">
         <v>35</v>
       </c>
@@ -1829,7 +1841,7 @@
       <c r="I37" s="6"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="46"/>
+      <c r="A38" s="56"/>
       <c r="B38" s="11" t="s">
         <v>34</v>
       </c>
@@ -1850,7 +1862,7 @@
       <c r="I38" s="6"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="46"/>
+      <c r="A39" s="56"/>
       <c r="B39" s="11" t="s">
         <v>28</v>
       </c>
@@ -1871,7 +1883,7 @@
       <c r="I39" s="6"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="46"/>
+      <c r="A40" s="56"/>
       <c r="B40" s="11" t="s">
         <v>11</v>
       </c>
@@ -1892,18 +1904,18 @@
       <c r="I40" s="6"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="45"/>
-      <c r="B41" s="45"/>
-      <c r="C41" s="45"/>
-      <c r="D41" s="45"/>
-      <c r="E41" s="45"/>
-      <c r="F41" s="45"/>
+      <c r="A41" s="55"/>
+      <c r="B41" s="55"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="55"/>
+      <c r="F41" s="55"/>
       <c r="G41" s="13"/>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
     </row>
     <row r="42" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="47" t="s">
+      <c r="A42" s="57" t="s">
         <v>32</v>
       </c>
       <c r="B42" s="11" t="s">
@@ -1926,7 +1938,7 @@
       <c r="I42" s="6"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="47"/>
+      <c r="A43" s="57"/>
       <c r="B43" s="11" t="s">
         <v>6</v>
       </c>
@@ -1947,7 +1959,7 @@
       <c r="I43" s="6"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="47"/>
+      <c r="A44" s="57"/>
       <c r="B44" s="11" t="s">
         <v>36</v>
       </c>
@@ -1968,7 +1980,7 @@
       <c r="I44" s="6"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="47"/>
+      <c r="A45" s="57"/>
       <c r="B45" s="11" t="s">
         <v>37</v>
       </c>
@@ -1989,7 +2001,7 @@
       <c r="I45" s="6"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="47"/>
+      <c r="A46" s="57"/>
       <c r="B46" s="11"/>
       <c r="C46" s="12"/>
       <c r="D46" s="12"/>
@@ -2096,17 +2108,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A33:A40"/>
+    <mergeCell ref="A42:A46"/>
+    <mergeCell ref="A10:A18"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A3:A8"/>
     <mergeCell ref="A20:A31"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A33:A40"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="A10:A18"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2128,15 +2140,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2162,8 +2174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F1C7CD-19A3-4E4C-8995-F8BF8AD34968}">
   <dimension ref="A2:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2195,7 +2207,7 @@
       <c r="D3" s="28"/>
     </row>
     <row r="4" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="60" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="32">
@@ -2209,7 +2221,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="55"/>
+      <c r="A5" s="60"/>
       <c r="B5" s="32">
         <v>1.1000000000000001</v>
       </c>
@@ -2219,7 +2231,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="55"/>
+      <c r="A6" s="60"/>
       <c r="B6" s="32">
         <v>1.2</v>
       </c>
@@ -2229,7 +2241,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="55"/>
+      <c r="A7" s="60"/>
       <c r="B7" s="32">
         <v>1.3</v>
       </c>
@@ -2239,7 +2251,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="55"/>
+      <c r="A8" s="60"/>
       <c r="B8" s="32">
         <v>1.4</v>
       </c>
@@ -2249,7 +2261,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="55"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="32">
         <v>1.5</v>
       </c>
@@ -2259,7 +2271,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="55"/>
+      <c r="A10" s="60"/>
       <c r="B10" s="32">
         <v>1.6</v>
       </c>
@@ -2269,7 +2281,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="55"/>
+      <c r="A11" s="60"/>
       <c r="B11" s="32">
         <v>1.7</v>
       </c>
@@ -2279,7 +2291,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="55"/>
+      <c r="A12" s="60"/>
       <c r="B12" s="32">
         <v>1.8</v>
       </c>
@@ -2289,7 +2301,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="55"/>
+      <c r="A13" s="60"/>
       <c r="B13" s="34">
         <v>2</v>
       </c>
@@ -2301,7 +2313,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="55"/>
+      <c r="A14" s="60"/>
       <c r="B14" s="34">
         <v>2.1</v>
       </c>
@@ -2311,7 +2323,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="55"/>
+      <c r="A15" s="60"/>
       <c r="B15" s="34">
         <v>2.2000000000000002</v>
       </c>
@@ -2321,7 +2333,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="55"/>
+      <c r="A16" s="60"/>
       <c r="B16" s="34">
         <v>3</v>
       </c>
@@ -2331,7 +2343,7 @@
       <c r="D16" s="33"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="55"/>
+      <c r="A17" s="60"/>
       <c r="B17" s="34">
         <v>3.1</v>
       </c>
@@ -2341,7 +2353,7 @@
       <c r="D17" s="33"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="55"/>
+      <c r="A18" s="60"/>
       <c r="B18" s="34">
         <v>3.2</v>
       </c>
@@ -2351,7 +2363,7 @@
       <c r="D18" s="33"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="55"/>
+      <c r="A19" s="60"/>
       <c r="B19" s="34">
         <v>4</v>
       </c>
@@ -2361,7 +2373,7 @@
       <c r="D19" s="33"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="55"/>
+      <c r="A20" s="60"/>
       <c r="B20" s="34">
         <v>4.0999999999999996</v>
       </c>
@@ -2371,7 +2383,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="55"/>
+      <c r="A21" s="60"/>
       <c r="B21" s="34">
         <v>4.2</v>
       </c>
@@ -2381,7 +2393,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="55"/>
+      <c r="A22" s="60"/>
       <c r="B22" s="34">
         <v>4.3</v>
       </c>
@@ -2391,7 +2403,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="55"/>
+      <c r="A23" s="60"/>
       <c r="B23" s="34">
         <v>4.4000000000000004</v>
       </c>
@@ -2401,7 +2413,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="55"/>
+      <c r="A24" s="60"/>
       <c r="B24" s="34"/>
       <c r="C24" s="35" t="s">
         <v>110</v>
@@ -2409,7 +2421,7 @@
       <c r="D24" s="33"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="55"/>
+      <c r="A25" s="60"/>
       <c r="B25" s="34"/>
       <c r="C25" s="35"/>
       <c r="D25" s="33" t="s">
@@ -2417,7 +2429,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="55"/>
+      <c r="A26" s="60"/>
       <c r="B26" s="34"/>
       <c r="C26" s="35"/>
       <c r="D26" s="33" t="s">
@@ -2425,7 +2437,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="55"/>
+      <c r="A27" s="60"/>
       <c r="B27" s="34"/>
       <c r="C27" s="35"/>
       <c r="D27" s="33" t="s">
@@ -2433,37 +2445,45 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="55"/>
+      <c r="A28" s="60"/>
       <c r="B28" s="34"/>
-      <c r="C28" s="35"/>
+      <c r="C28" s="35" t="s">
+        <v>124</v>
+      </c>
       <c r="D28" s="33"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="55"/>
+      <c r="A29" s="60"/>
       <c r="B29" s="34"/>
-      <c r="C29" s="35"/>
+      <c r="C29" s="35" t="s">
+        <v>125</v>
+      </c>
       <c r="D29" s="33"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="55"/>
+      <c r="A30" s="60"/>
       <c r="B30" s="34"/>
-      <c r="C30" s="35"/>
+      <c r="C30" s="35" t="s">
+        <v>126</v>
+      </c>
       <c r="D30" s="33"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="55"/>
+      <c r="A31" s="60"/>
       <c r="B31" s="34"/>
-      <c r="C31" s="35"/>
+      <c r="C31" s="35" t="s">
+        <v>127</v>
+      </c>
       <c r="D31" s="33"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="57"/>
-      <c r="B32" s="57"/>
-      <c r="C32" s="57"/>
-      <c r="D32" s="57"/>
+      <c r="A32" s="62"/>
+      <c r="B32" s="62"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="62"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="56" t="s">
+      <c r="A33" s="61" t="s">
         <v>33</v>
       </c>
       <c r="B33" s="37">
@@ -2475,7 +2495,7 @@
       <c r="D33" s="39"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="56"/>
+      <c r="A34" s="61"/>
       <c r="B34" s="37">
         <v>5</v>
       </c>
@@ -2485,7 +2505,7 @@
       <c r="D34" s="39"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="56"/>
+      <c r="A35" s="61"/>
       <c r="B35" s="37">
         <v>6</v>
       </c>
@@ -2495,7 +2515,7 @@
       <c r="D35" s="39"/>
     </row>
     <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="56"/>
+      <c r="A36" s="61"/>
       <c r="B36" s="37">
         <v>7</v>
       </c>
@@ -2505,7 +2525,7 @@
       <c r="D36" s="39"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="56"/>
+      <c r="A37" s="61"/>
       <c r="B37" s="37">
         <v>8</v>
       </c>
@@ -2517,7 +2537,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="56"/>
+      <c r="A38" s="61"/>
       <c r="B38" s="37">
         <v>8.1</v>
       </c>
@@ -2527,7 +2547,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="56"/>
+      <c r="A39" s="61"/>
       <c r="B39" s="37">
         <v>8.1999999999999993</v>
       </c>
@@ -2537,7 +2557,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="56"/>
+      <c r="A40" s="61"/>
       <c r="B40" s="37">
         <v>8.3000000000000007</v>
       </c>
@@ -2547,7 +2567,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="56"/>
+      <c r="A41" s="61"/>
       <c r="B41" s="37">
         <v>8.4</v>
       </c>
@@ -2557,7 +2577,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="56"/>
+      <c r="A42" s="61"/>
       <c r="B42" s="37">
         <v>8.5</v>
       </c>
@@ -2573,7 +2593,7 @@
       <c r="D43" s="27"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="54" t="s">
+      <c r="A44" s="59" t="s">
         <v>93</v>
       </c>
       <c r="B44" s="40">
@@ -2585,7 +2605,7 @@
       <c r="D44" s="42"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="54"/>
+      <c r="A45" s="59"/>
       <c r="B45" s="40">
         <v>10</v>
       </c>
@@ -2595,7 +2615,7 @@
       <c r="D45" s="42"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="54"/>
+      <c r="A46" s="59"/>
       <c r="B46" s="40">
         <v>11</v>
       </c>
@@ -2605,7 +2625,7 @@
       <c r="D46" s="42"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="54"/>
+      <c r="A47" s="59"/>
       <c r="B47" s="40">
         <v>12</v>
       </c>
@@ -2615,7 +2635,7 @@
       <c r="D47" s="42"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="54"/>
+      <c r="A48" s="59"/>
       <c r="B48" s="40">
         <v>13</v>
       </c>
@@ -2625,7 +2645,7 @@
       <c r="D48" s="42"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="54"/>
+      <c r="A49" s="59"/>
       <c r="B49" s="40">
         <v>14</v>
       </c>
@@ -2641,174 +2661,174 @@
       <c r="D50" s="27"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="61" t="s">
+      <c r="A51" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="B51" s="58">
+      <c r="B51" s="43">
         <v>1</v>
       </c>
-      <c r="C51" s="59" t="s">
+      <c r="C51" s="44" t="s">
         <v>105</v>
       </c>
-      <c r="D51" s="60"/>
+      <c r="D51" s="45"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="61"/>
-      <c r="B52" s="58">
+      <c r="A52" s="63"/>
+      <c r="B52" s="43">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C52" s="59"/>
-      <c r="D52" s="60" t="s">
+      <c r="C52" s="44"/>
+      <c r="D52" s="45" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="61"/>
-      <c r="B53" s="58">
+      <c r="A53" s="63"/>
+      <c r="B53" s="43">
         <v>1.2</v>
       </c>
-      <c r="C53" s="59"/>
-      <c r="D53" s="60" t="s">
+      <c r="C53" s="44"/>
+      <c r="D53" s="45" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="61"/>
-      <c r="B54" s="58">
+      <c r="A54" s="63"/>
+      <c r="B54" s="43">
         <v>1.3</v>
       </c>
-      <c r="C54" s="59"/>
-      <c r="D54" s="60" t="s">
+      <c r="C54" s="44"/>
+      <c r="D54" s="45" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="61"/>
-      <c r="B55" s="58"/>
-      <c r="C55" s="59"/>
-      <c r="D55" s="60" t="s">
+      <c r="A55" s="63"/>
+      <c r="B55" s="43"/>
+      <c r="C55" s="44"/>
+      <c r="D55" s="45" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="61"/>
-      <c r="B56" s="58"/>
-      <c r="C56" s="59" t="s">
+      <c r="A56" s="63"/>
+      <c r="B56" s="43"/>
+      <c r="C56" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="D56" s="60"/>
+      <c r="D56" s="45"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="61"/>
-      <c r="B57" s="58"/>
-      <c r="C57" s="59"/>
-      <c r="D57" s="60" t="s">
+      <c r="A57" s="63"/>
+      <c r="B57" s="43"/>
+      <c r="C57" s="44"/>
+      <c r="D57" s="45" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="61"/>
-      <c r="B58" s="58"/>
-      <c r="C58" s="59"/>
-      <c r="D58" s="63" t="s">
+      <c r="A58" s="63"/>
+      <c r="B58" s="43"/>
+      <c r="C58" s="44"/>
+      <c r="D58" s="47" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="61"/>
-      <c r="B59" s="58">
+      <c r="A59" s="63"/>
+      <c r="B59" s="43">
         <v>2</v>
       </c>
-      <c r="C59" s="59" t="s">
+      <c r="C59" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="D59" s="60"/>
+      <c r="D59" s="45"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="61"/>
-      <c r="B60" s="58"/>
-      <c r="C60" s="59"/>
-      <c r="D60" s="60" t="s">
+      <c r="A60" s="63"/>
+      <c r="B60" s="43"/>
+      <c r="C60" s="44"/>
+      <c r="D60" s="45" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="61"/>
-      <c r="B61" s="58"/>
-      <c r="C61" s="59"/>
-      <c r="D61" s="60" t="s">
+      <c r="A61" s="63"/>
+      <c r="B61" s="43"/>
+      <c r="C61" s="44"/>
+      <c r="D61" s="45" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="61"/>
-      <c r="B62" s="58"/>
-      <c r="C62" s="59"/>
-      <c r="D62" s="60" t="s">
+      <c r="A62" s="63"/>
+      <c r="B62" s="43"/>
+      <c r="C62" s="44"/>
+      <c r="D62" s="45" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="61"/>
-      <c r="B63" s="58">
+      <c r="A63" s="63"/>
+      <c r="B63" s="43">
         <v>3</v>
       </c>
-      <c r="C63" s="59" t="s">
+      <c r="C63" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="D63" s="60"/>
+      <c r="D63" s="45"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="61"/>
-      <c r="B64" s="58"/>
-      <c r="C64" s="59" t="s">
+      <c r="A64" s="63"/>
+      <c r="B64" s="43"/>
+      <c r="C64" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="D64" s="60"/>
+      <c r="D64" s="45"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="61"/>
-      <c r="B65" s="58">
+      <c r="A65" s="63"/>
+      <c r="B65" s="43">
         <v>4</v>
       </c>
-      <c r="C65" s="59" t="s">
+      <c r="C65" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="D65" s="60"/>
+      <c r="D65" s="45"/>
     </row>
     <row r="66" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="61"/>
-      <c r="B66" s="58">
+      <c r="A66" s="63"/>
+      <c r="B66" s="43">
         <v>5</v>
       </c>
-      <c r="C66" s="62" t="s">
+      <c r="C66" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="D66" s="60" t="s">
+      <c r="D66" s="45" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="61"/>
-      <c r="B67" s="58"/>
-      <c r="C67" s="59"/>
-      <c r="D67" s="60" t="s">
+      <c r="A67" s="63"/>
+      <c r="B67" s="43"/>
+      <c r="C67" s="44"/>
+      <c r="D67" s="45" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="61"/>
-      <c r="B68" s="58"/>
-      <c r="C68" s="59"/>
-      <c r="D68" s="60" t="s">
+      <c r="A68" s="63"/>
+      <c r="B68" s="43"/>
+      <c r="C68" s="44"/>
+      <c r="D68" s="45" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="61"/>
-      <c r="B69" s="58"/>
-      <c r="C69" s="59"/>
-      <c r="D69" s="60"/>
+      <c r="A69" s="63"/>
+      <c r="B69" s="43"/>
+      <c r="C69" s="44"/>
+      <c r="D69" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>